<commit_message>
updated answer key for unit 3 assessment
</commit_message>
<xml_diff>
--- a/unit_assements/3_Databases/answer_key.xlsx
+++ b/unit_assements/3_Databases/answer_key.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\vyu\Documents\data_bootcamp\MyRepo\data-bootcamp-activities\unit_assements\3_Databases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D093AEF8-3D90-4BF4-8029-E3B30A8BD40E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-28920" yWindow="6720" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,6 +72,539 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>411249</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>163570</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5037E732-0736-4B8B-BF13-7054C40A8DE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11993649" cy="11784070"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>316496</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>153910</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9433EF2F-2B8B-4E4E-872F-D0A701FD9050}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="11811000"/>
+          <a:ext cx="15556496" cy="10821910"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>298209</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>68359</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11C89BE2-A608-4E61-85C7-A63FF2F45BDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="25908000"/>
+          <a:ext cx="21024609" cy="12069859"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>336314</xdr:colOff>
+      <xdr:row>254</xdr:row>
+      <xdr:rowOff>144384</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BD31738-EC88-4C0A-BE4C-A04FFBAC0FE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="38100000"/>
+          <a:ext cx="21062714" cy="10812384"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>255</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>326788</xdr:colOff>
+      <xdr:row>305</xdr:row>
+      <xdr:rowOff>20382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ED7CFD7-52C6-4012-B929-82138A5D99E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="48958500"/>
+          <a:ext cx="21053188" cy="9545382"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>336314</xdr:colOff>
+      <xdr:row>355</xdr:row>
+      <xdr:rowOff>39408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA117561-0D3B-43ED-B2D2-D11C34914396}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="58674000"/>
+          <a:ext cx="21062714" cy="9373908"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>356</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>362851</xdr:colOff>
+      <xdr:row>401</xdr:row>
+      <xdr:rowOff>163144</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F34FC9C5-F4D6-4A95-A36F-4DD68E2FE5E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="68199000"/>
+          <a:ext cx="6458851" cy="8735644"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>402</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>336229</xdr:colOff>
+      <xdr:row>445</xdr:row>
+      <xdr:rowOff>58301</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B70D381B-45C8-4645-AF3E-5D1155E97E51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="76962000"/>
+          <a:ext cx="20453029" cy="8249801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>446</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>67620</xdr:colOff>
+      <xdr:row>490</xdr:row>
+      <xdr:rowOff>172644</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3D0EE51-6CD8-45AE-BFEA-816FE19B0B24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="85344000"/>
+          <a:ext cx="6773220" cy="8554644"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>491</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>553974</xdr:colOff>
+      <xdr:row>555</xdr:row>
+      <xdr:rowOff>173176</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CE856FE-A49C-49FE-8D3A-67F81F68FFE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="93916500"/>
+          <a:ext cx="10917174" cy="12365176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>556</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>229653</xdr:colOff>
+      <xdr:row>577</xdr:row>
+      <xdr:rowOff>124401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35C389B4-F9D1-49E5-9220-A98FD3C45D40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="106299000"/>
+          <a:ext cx="7544853" cy="4124901"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>353240</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>67049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24839EA1-2A1D-416F-965F-B33763756174}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="22726650"/>
+          <a:ext cx="5839640" cy="2676899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +869,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="L126" sqref="L126"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>